<commit_message>
updated inventory and rookie decks
</commit_message>
<xml_diff>
--- a/decks/rookie_decks.xlsx
+++ b/decks/rookie_decks.xlsx
@@ -15,7 +15,7 @@
     <sheet name="blue" sheetId="1" r:id="rId1"/>
     <sheet name="red" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -941,7 +941,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,11 +989,11 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D12" si="0">B3-C3</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1091,11 +1091,11 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1142,6 +1142,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1258,11 +1261,11 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,11 +1306,11 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
purchased cards for rookie decks at dsg
</commit_message>
<xml_diff>
--- a/decks/rookie_decks.xlsx
+++ b/decks/rookie_decks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="8910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="blue" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,11 +1201,11 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1216,11 +1216,11 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,11 +1246,11 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1291,11 +1291,11 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>